<commit_message>
polished table a bit
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasvietto/Documents/Data Viz/Table Contest 24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasvietto/Documents/GitHub Pushed Projects/Table Contest 2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6A5876-945A-C142-A6B7-063E87185254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21BDC9D-C898-8B47-A553-C2E691E2D12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3B4B8E8F-10E9-A64B-A13C-0E47E1EDDE36}"/>
   </bookViews>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83074F10-FA98-CE46-90A3-2DF5AD16E04C}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,7 +1510,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>43</v>

</xml_diff>